<commit_message>
Added all missing data to MasterCollection, added MultiTracksTop120 to CcliTop100.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/CcwsBethelCommunity/CcwsBethelCommunity.xlsx
+++ b/WorshipCreator.TestData/Source/Books/CcwsBethelCommunity/CcwsBethelCommunity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\CcwsBethelCommunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93522025-EB05-4AA1-8ED7-7654F94A131B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC96848-B015-4CDC-B39E-F185B2D6B0C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Final V1" guid="{3D90CCC9-2098-49D0-B048-150589B000BB}" includePrintSettings="0" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
+    <customWorkbookView name="Changes for V2" guid="{FC34F940-3EA4-4915-AF37-108B14C951B2}" includePrintSettings="0" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
     <customWorkbookView name="Transpose for V2" guid="{7CF7E09B-DE34-46B0-A744-0543B6C0C399}" includePrintSettings="0" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
-    <customWorkbookView name="Changes for V2" guid="{FC34F940-3EA4-4915-AF37-108B14C951B2}" includePrintSettings="0" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
-    <customWorkbookView name="Final V1" guid="{3D90CCC9-2098-49D0-B048-150589B000BB}" includePrintSettings="0" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">

</xml_diff>